<commit_message>
adapted data excel file for dataSufficiency
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/13_data_sufficiency/20240613_Datenmodel_DataSufficiency.xlsx
+++ b/02_work_doc/01_daten/13_data_sufficiency/20240613_Datenmodel_DataSufficiency.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="20240613_Datenmodel_Datensuffiz" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="20240613_Datenmodel_Datensuffiz" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,6 +40,15 @@
     <t xml:space="preserve">Beispiel_2</t>
   </si>
   <si>
+    <t xml:space="preserve">Beispiel_1_Überschrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beispiel_2_Überschrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Literatur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zustandsbeobachter</t>
   </si>
   <si>
@@ -55,7 +64,13 @@
     <t xml:space="preserve">Durch die Diskretisierung von kontinuierlichen Signalen oder Daten können sie in diskrete Intervalle oder Kategorien unterteilt werden. Dies reduziert die Datenfrequenz, indem kontinuierliche Daten in diskrete Werte umgewandelt werden, was oft ausreicht, um wichtige Informationen zu erhalten.</t>
   </si>
   <si>
-    <t xml:space="preserve">Anstatt kontinuierliche Daten aufzuzeichnen, können nur relevante Ereignisse oder Zustandsänderungen aufgezeichnet werden.</t>
+    <t xml:space="preserve">Beispiel 1 Überschrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beispiel 2 Überschrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arndt, Henrik (2006): Integrierte Informationsarchitektur. Die erfolgreiche Konzeption professioneller Websites. Berlin, Heidelberg: Springer.;;Grzyb, Kai Robin, Alexander Rösler, Jana Rockstroh, Torsten Bartel und Gesine Quint (2016): Eye Tracking in Usability-Tests: Ein Mehrwert auch in rein qualitativen Studien, hg. v. S. Hess und H. Fischer. Veranstaltung: Mensch und Computer 2016 - Usability Professionals, Aachen. &lt;a href="https://dl.gi.de/server/api/core/bitstreams/968aa227-06a7-4ec6-981f-3353b7d67e01/content"&gt;https://dl.gi.de/server/api/core/bitstreams/968aa227-06a7-4ec6-981f-3353b7d67e01/content&lt;/a&gt;;;Maas, Jörg (2011): Werbewirkungsforschung. In: Qualitative Marktforschung in Theorie und Praxis, hg. v. Gabriele Naderer und Eva Balzer, S. 519–536. Wiesbaden: Gabler.((Maas_2011));;Müller, Karsten, Julia David und Tammo Straatmann (2011): Qualitative Beobachtungsverfahren. In: Qualitative Marktforschung in Theorie und Praxis, hg. v. Gabriele Naderer und Eva Balzer, S. 313–344. Wiesbaden: Gabler.</t>
   </si>
   <si>
     <t xml:space="preserve">Reduzierung der Datenfrequenz</t>
@@ -86,11 +101,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,6 +122,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,8 +172,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -167,112 +201,238 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="295.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="239.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="104.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="295.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="239.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="104.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>14</v>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>17</v>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>18</v>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://dl.gi.de/server/api/core/bitstreams/968aa227"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>